<commit_message>
Se añadio la tasa de ausentismo
</commit_message>
<xml_diff>
--- a/Paquete/Database.xlsx
+++ b/Paquete/Database.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="mv" sheetId="1" state="visible" r:id="rId2"/>
@@ -96,8 +96,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -118,31 +122,72 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C37"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A21" activeCellId="0" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="n">
+      <c r="A1" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="B1" s="0" t="n">
+      <c r="B1" s="1" t="n">
         <v>5</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
+      <c r="A2" s="1" t="n">
         <v>50000</v>
       </c>
-      <c r="B2" s="0" t="n">
+      <c r="B2" s="1" t="n">
         <v>200000</v>
       </c>
-      <c r="C2" t="n" s="0">
+      <c r="C2" s="1" t="n">
         <v>0.25</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="1" t="n">
+        <v>1750</v>
+      </c>
+      <c r="B20" s="1" t="n">
+        <v>1750</v>
+      </c>
+      <c r="C20" s="1" t="n">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="1" t="n">
+        <v>1750</v>
+      </c>
+      <c r="B21" s="1" t="n">
+        <v>1750</v>
+      </c>
+      <c r="C21" s="1" t="n">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="1" t="n">
+        <v>1750</v>
+      </c>
+      <c r="B22" s="1" t="n">
+        <v>1750</v>
+      </c>
+      <c r="C22" s="1" t="n">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B37" s="1" t="n">
+        <v>500</v>
+      </c>
+      <c r="C37" s="1" t="n">
+        <v>300</v>
       </c>
     </row>
   </sheetData>
@@ -184,20 +229,34 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B23" activeCellId="0" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="n">
+      <c r="A1" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B1" s="0" t="n">
+      <c r="B1" s="1" t="n">
         <v>2</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="1" t="n">
+        <v>1750</v>
+      </c>
+      <c r="B21" s="1" t="n">
+        <v>1750</v>
+      </c>
+      <c r="C21" s="1" t="n">
+        <v>800</v>
+      </c>
+      <c r="E21" t="n" s="0">
+        <v>200.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>